<commit_message>
热管 Signed-off-by: tuchengen <tuchengen@qq.com>
</commit_message>
<xml_diff>
--- a/桩基计算/输电线路桩基公式（2021.10.29）.xlsx
+++ b/桩基计算/输电线路桩基公式（2021.10.29）.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540"/>
+    <workbookView windowWidth="6615" windowHeight="1530"/>
   </bookViews>
   <sheets>
     <sheet name="低桩承台" sheetId="1" r:id="rId1"/>
@@ -1026,15 +1026,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="9">
+    <numFmt numFmtId="176" formatCode="0.0_ "/>
+    <numFmt numFmtId="177" formatCode="0.000_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="0.0_ "/>
+    <numFmt numFmtId="178" formatCode="0.00000_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.00_ "/>
-    <numFmt numFmtId="178" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="179" formatCode="0.000_ "/>
-    <numFmt numFmtId="180" formatCode="0.00000_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="0.00_ "/>
+    <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
   <fonts count="39">
     <font>
@@ -1098,6 +1098,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -1113,7 +1121,60 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1127,53 +1188,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1187,56 +1235,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1336,7 +1336,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1348,7 +1354,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1360,13 +1366,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1378,43 +1468,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1426,97 +1516,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1694,21 +1694,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1719,15 +1704,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1749,11 +1725,42 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1775,18 +1782,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1798,10 +1798,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1810,137 +1810,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1989,7 +1989,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2025,7 +2025,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2085,58 +2085,52 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2207,7 +2201,57 @@
 </styleSheet>
 </file>
 
+<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" r:id="rId1" ax:persistence="persistStreamInit"/>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>38100</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>1085850</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>247650</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2050" name="计算" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2050"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14839950" y="381000"/>
+              <a:ext cx="1047750" cy="238125"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2627,7 +2671,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A32" sqref="$A29:$XFD32"/>
     </sheetView>
   </sheetViews>
@@ -2956,21 +3000,21 @@
         <v>24</v>
       </c>
       <c r="H15" s="35"/>
-      <c r="I15" s="61" t="s">
+      <c r="I15" s="47" t="s">
         <v>33</v>
       </c>
       <c r="J15" s="35"/>
-      <c r="K15" s="61" t="s">
+      <c r="K15" s="47" t="s">
         <v>34</v>
       </c>
       <c r="L15" s="35"/>
-      <c r="M15" s="61" t="s">
+      <c r="M15" s="47" t="s">
         <v>35</v>
       </c>
       <c r="N15" s="35"/>
     </row>
     <row r="16" ht="20.1" customHeight="1" spans="1:14">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="44" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="35"/>
@@ -2986,34 +3030,34 @@
         <v>24</v>
       </c>
       <c r="H16" s="35"/>
-      <c r="I16" s="61" t="s">
+      <c r="I16" s="47" t="s">
         <v>33</v>
       </c>
       <c r="J16" s="35"/>
-      <c r="K16" s="61" t="s">
+      <c r="K16" s="47" t="s">
         <v>34</v>
       </c>
       <c r="L16" s="35"/>
-      <c r="M16" s="61" t="s">
+      <c r="M16" s="47" t="s">
         <v>35</v>
       </c>
       <c r="N16" s="35"/>
     </row>
     <row r="17" ht="20.1" customHeight="1" spans="1:14">
-      <c r="A17" s="50"/>
-      <c r="B17" s="50"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
       <c r="C17" s="44"/>
-      <c r="D17" s="50"/>
+      <c r="D17" s="44"/>
       <c r="E17" s="47"/>
-      <c r="F17" s="50"/>
+      <c r="F17" s="44"/>
       <c r="G17" s="44"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="50"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="61"/>
-      <c r="N17" s="50"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="44"/>
     </row>
     <row r="18" ht="20.1" customHeight="1" spans="1:14">
       <c r="A18" s="45" t="s">
@@ -3021,20 +3065,20 @@
       </c>
       <c r="B18" s="46"/>
       <c r="C18" s="44"/>
-      <c r="D18" s="50"/>
+      <c r="D18" s="44"/>
       <c r="E18" s="47"/>
-      <c r="F18" s="50"/>
+      <c r="F18" s="44"/>
       <c r="G18" s="44"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="61"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="61"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="61"/>
-      <c r="N18" s="50"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="44"/>
     </row>
     <row r="19" ht="20.1" customHeight="1" spans="1:14">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="44" t="s">
         <v>40</v>
       </c>
       <c r="B19" s="35">
@@ -3053,121 +3097,121 @@
         <v>3</v>
       </c>
       <c r="G19" s="44"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="61"/>
-      <c r="N19" s="50"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="44"/>
     </row>
     <row r="20" ht="20.1" customHeight="1" spans="1:14">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="50">
+      <c r="B20" s="44">
         <v>1</v>
       </c>
       <c r="C20" s="44">
         <v>2</v>
       </c>
-      <c r="D20" s="50">
+      <c r="D20" s="44">
         <v>3</v>
       </c>
       <c r="E20" s="47">
         <v>4</v>
       </c>
-      <c r="F20" s="50">
+      <c r="F20" s="44">
         <v>5</v>
       </c>
       <c r="G20" s="44">
         <v>6</v>
       </c>
-      <c r="H20" s="50">
+      <c r="H20" s="44">
         <v>7</v>
       </c>
-      <c r="I20" s="61">
+      <c r="I20" s="47">
         <v>8</v>
       </c>
-      <c r="J20" s="50">
+      <c r="J20" s="44">
         <v>9</v>
       </c>
-      <c r="K20" s="61"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="61"/>
-      <c r="N20" s="50"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="44"/>
     </row>
     <row r="21" ht="20.1" customHeight="1" spans="1:14">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="50">
+      <c r="B21" s="44">
         <v>3</v>
       </c>
       <c r="C21" s="44">
         <v>3</v>
       </c>
-      <c r="D21" s="50">
+      <c r="D21" s="44">
         <v>3</v>
       </c>
       <c r="E21" s="47">
         <v>0</v>
       </c>
-      <c r="F21" s="50">
+      <c r="F21" s="44">
         <v>0</v>
       </c>
       <c r="G21" s="44">
         <v>0</v>
       </c>
-      <c r="H21" s="50">
+      <c r="H21" s="44">
         <v>-3</v>
       </c>
-      <c r="I21" s="61">
+      <c r="I21" s="47">
         <v>-3</v>
       </c>
-      <c r="J21" s="50">
+      <c r="J21" s="44">
         <v>-3</v>
       </c>
-      <c r="K21" s="61"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="61"/>
-      <c r="N21" s="50"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="44"/>
     </row>
     <row r="22" ht="20.1" customHeight="1" spans="1:14">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="50">
+      <c r="B22" s="44">
         <v>3</v>
       </c>
       <c r="C22" s="44">
         <v>0</v>
       </c>
-      <c r="D22" s="50">
+      <c r="D22" s="44">
         <v>-3</v>
       </c>
       <c r="E22" s="47">
         <v>-3</v>
       </c>
-      <c r="F22" s="50">
+      <c r="F22" s="44">
         <v>0</v>
       </c>
       <c r="G22" s="44">
         <v>3</v>
       </c>
-      <c r="H22" s="50">
+      <c r="H22" s="44">
         <v>3</v>
       </c>
-      <c r="I22" s="61">
-        <v>0</v>
-      </c>
-      <c r="J22" s="50">
+      <c r="I22" s="47">
+        <v>0</v>
+      </c>
+      <c r="J22" s="44">
         <v>-3</v>
       </c>
-      <c r="K22" s="61"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="61"/>
-      <c r="N22" s="50"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="44"/>
     </row>
     <row r="23" ht="20.1" customHeight="1" spans="1:7">
       <c r="A23" s="42"/>
@@ -3239,7 +3283,7 @@
       <c r="G26" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="51">
+      <c r="H26" s="50">
         <f>PI()*B25^2/4</f>
         <v>3.14159265358979</v>
       </c>
@@ -3267,14 +3311,14 @@
       <c r="E27" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="52">
+      <c r="F27" s="51">
         <f>(B26*PI()*D26^2/4)/(PI()*B25*B25*1000*1000/4)</f>
         <v>0.00875</v>
       </c>
       <c r="G27" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="H27" s="51">
+      <c r="H27" s="50">
         <f>PI()*B25</f>
         <v>6.28318530717959</v>
       </c>
@@ -3313,7 +3357,7 @@
     </row>
     <row r="33" ht="20.1" customHeight="1"/>
     <row r="34" ht="20.1" customHeight="1" spans="1:1">
-      <c r="A34" s="53" t="s">
+      <c r="A34" s="52" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3330,43 +3374,43 @@
       <c r="D35" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="E35" s="54" t="s">
+      <c r="E35" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="F35" s="54" t="s">
+      <c r="F35" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="G35" s="54" t="s">
+      <c r="G35" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="H35" s="54" t="s">
+      <c r="H35" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="I35" s="54" t="s">
+      <c r="I35" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="J35" s="54" t="s">
+      <c r="J35" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="K35" s="54" t="s">
+      <c r="K35" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="L35" s="54" t="s">
+      <c r="L35" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="M35" s="54" t="s">
+      <c r="M35" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="N35" s="54" t="s">
+      <c r="N35" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="O35" s="54" t="s">
+      <c r="O35" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="P35" s="54" t="s">
+      <c r="P35" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="Q35" s="54" t="s">
+      <c r="Q35" s="53" t="s">
         <v>79</v>
       </c>
     </row>
@@ -3402,31 +3446,31 @@
         <f t="shared" ref="J36:J45" si="0">VLOOKUP(B36,土设计参数,2,FALSE)</f>
         <v>0.7</v>
       </c>
-      <c r="K36" s="51">
+      <c r="K36" s="50">
         <f t="shared" ref="K36:K45" si="1">VLOOKUP(B36,土设计参数,3,FALSE)</f>
         <v>0.832553207401873</v>
       </c>
-      <c r="L36" s="51">
+      <c r="L36" s="50">
         <f t="shared" ref="L36:L45" si="2">VLOOKUP(B36,土设计参数,4,FALSE)</f>
         <v>0.795270728767051</v>
       </c>
-      <c r="M36" s="62">
+      <c r="M36" s="60">
         <f>SUM(D36)</f>
         <v>25</v>
       </c>
-      <c r="N36" s="62">
+      <c r="N36" s="60">
         <f>IF($M36&lt;=$F$25,D36,$F$25-0)</f>
         <v>14.7</v>
       </c>
-      <c r="O36" s="63">
+      <c r="O36" s="61">
         <f t="shared" ref="O36:O45" si="3">IF(N36=0,0,$H$27*K36*N36*E36)</f>
         <v>1691.73323833432</v>
       </c>
-      <c r="P36" s="63">
+      <c r="P36" s="61">
         <f t="shared" ref="P36:P45" si="4">IF(N36=0,0,$H$27*J36*N36*E36)</f>
         <v>1422.38748983931</v>
       </c>
-      <c r="Q36" s="65">
+      <c r="Q36" s="63">
         <f t="shared" ref="Q36:Q45" si="5">$H$26*L36*F36</f>
         <v>0</v>
       </c>
@@ -3463,31 +3507,31 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="K37" s="51">
+      <c r="K37" s="50">
         <f t="shared" si="1"/>
         <v>0.736808550160793</v>
       </c>
-      <c r="L37" s="51">
+      <c r="L37" s="50">
         <f t="shared" si="2"/>
         <v>0.736808550160793</v>
       </c>
-      <c r="M37" s="62">
+      <c r="M37" s="60">
         <f>SUM(D36:D37)</f>
         <v>26</v>
       </c>
-      <c r="N37" s="62">
+      <c r="N37" s="60">
         <f t="shared" ref="N37:N45" si="6">IF(M36&gt;$F$25,0,IF($M37&lt;=$F$25,D37,$F$25-M36))</f>
         <v>0</v>
       </c>
-      <c r="O37" s="63">
+      <c r="O37" s="61">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P37" s="63">
+      <c r="P37" s="61">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q37" s="65">
+      <c r="Q37" s="63">
         <f t="shared" si="5"/>
         <v>4629.50465657459</v>
       </c>
@@ -3524,31 +3568,31 @@
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="K38" s="51">
+      <c r="K38" s="50">
         <f t="shared" si="1"/>
         <v>0.832553207401873</v>
       </c>
-      <c r="L38" s="51">
+      <c r="L38" s="50">
         <f t="shared" si="2"/>
         <v>0.795270728767051</v>
       </c>
-      <c r="M38" s="62">
+      <c r="M38" s="60">
         <f>SUM(D36:D38)</f>
         <v>41</v>
       </c>
-      <c r="N38" s="62">
+      <c r="N38" s="60">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O38" s="63">
+      <c r="O38" s="61">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P38" s="63">
+      <c r="P38" s="61">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q38" s="65">
+      <c r="Q38" s="63">
         <f t="shared" si="5"/>
         <v>1998.73334328765</v>
       </c>
@@ -3569,31 +3613,31 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="K39" s="51" t="e">
+      <c r="K39" s="50" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="L39" s="51" t="e">
+      <c r="L39" s="50" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="M39" s="62">
+      <c r="M39" s="60">
         <f>SUM(D36:D39)</f>
         <v>41</v>
       </c>
-      <c r="N39" s="62">
+      <c r="N39" s="60">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O39" s="63">
+      <c r="O39" s="61">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P39" s="63">
+      <c r="P39" s="61">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q39" s="65" t="e">
+      <c r="Q39" s="63" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -3614,31 +3658,31 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="K40" s="51" t="e">
+      <c r="K40" s="50" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="L40" s="51" t="e">
+      <c r="L40" s="50" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="M40" s="62">
+      <c r="M40" s="60">
         <f>SUM(D36:D40)</f>
         <v>41</v>
       </c>
-      <c r="N40" s="62">
+      <c r="N40" s="60">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O40" s="63">
+      <c r="O40" s="61">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P40" s="63">
+      <c r="P40" s="61">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q40" s="65" t="e">
+      <c r="Q40" s="63" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -3659,31 +3703,31 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="K41" s="51" t="e">
+      <c r="K41" s="50" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="L41" s="51" t="e">
+      <c r="L41" s="50" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="M41" s="62">
+      <c r="M41" s="60">
         <f>SUM(D36:D41)</f>
         <v>41</v>
       </c>
-      <c r="N41" s="62">
+      <c r="N41" s="60">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O41" s="63">
+      <c r="O41" s="61">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P41" s="63">
+      <c r="P41" s="61">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q41" s="65" t="e">
+      <c r="Q41" s="63" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -3704,31 +3748,31 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="K42" s="51" t="e">
+      <c r="K42" s="50" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="L42" s="51" t="e">
+      <c r="L42" s="50" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="M42" s="62">
+      <c r="M42" s="60">
         <f>SUM(D36:D42)</f>
         <v>41</v>
       </c>
-      <c r="N42" s="62">
+      <c r="N42" s="60">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O42" s="63">
+      <c r="O42" s="61">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P42" s="63">
+      <c r="P42" s="61">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q42" s="65" t="e">
+      <c r="Q42" s="63" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -3749,31 +3793,31 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="K43" s="51" t="e">
+      <c r="K43" s="50" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="L43" s="51" t="e">
+      <c r="L43" s="50" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="M43" s="62">
+      <c r="M43" s="60">
         <f>SUM(D36:D43)</f>
         <v>41</v>
       </c>
-      <c r="N43" s="62">
+      <c r="N43" s="60">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O43" s="63">
+      <c r="O43" s="61">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P43" s="63">
+      <c r="P43" s="61">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q43" s="65" t="e">
+      <c r="Q43" s="63" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -3794,31 +3838,31 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="K44" s="51" t="e">
+      <c r="K44" s="50" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="L44" s="51" t="e">
+      <c r="L44" s="50" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="M44" s="62">
+      <c r="M44" s="60">
         <f>SUM(D36:D44)</f>
         <v>41</v>
       </c>
-      <c r="N44" s="62">
+      <c r="N44" s="60">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O44" s="63">
+      <c r="O44" s="61">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P44" s="63">
+      <c r="P44" s="61">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q44" s="65" t="e">
+      <c r="Q44" s="63" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -3839,196 +3883,196 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="K45" s="51" t="e">
+      <c r="K45" s="50" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="L45" s="51" t="e">
+      <c r="L45" s="50" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="M45" s="62">
+      <c r="M45" s="60">
         <f>SUM(D36:D45)</f>
         <v>41</v>
       </c>
-      <c r="N45" s="62">
+      <c r="N45" s="60">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O45" s="63">
+      <c r="O45" s="61">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P45" s="63">
+      <c r="P45" s="61">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q45" s="65" t="e">
+      <c r="Q45" s="63" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="46" ht="20.1" customHeight="1"/>
     <row r="47" ht="20.1" customHeight="1" spans="1:11">
-      <c r="A47" s="55" t="s">
+      <c r="A47" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="B47" s="56"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
-      <c r="H47" s="56"/>
-      <c r="K47" s="64"/>
+      <c r="B47" s="55"/>
+      <c r="C47" s="55"/>
+      <c r="D47" s="55"/>
+      <c r="E47" s="55"/>
+      <c r="F47" s="55"/>
+      <c r="G47" s="55"/>
+      <c r="H47" s="55"/>
+      <c r="K47" s="62"/>
     </row>
     <row r="48" ht="20.1" customHeight="1" spans="1:8">
       <c r="A48" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="57">
+      <c r="B48" s="56">
         <f>B7+24*H26*D25</f>
         <v>-229.973125486746</v>
       </c>
       <c r="C48" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="D48" s="57">
+      <c r="D48" s="56">
         <f>SUM(P36:P45)</f>
         <v>1422.38748983931</v>
       </c>
-      <c r="E48" s="56"/>
-      <c r="F48" s="56"/>
-      <c r="G48" s="56"/>
-      <c r="H48" s="56"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="55"/>
+      <c r="G48" s="55"/>
+      <c r="H48" s="55"/>
     </row>
     <row r="49" ht="20.1" customHeight="1" spans="1:8">
       <c r="A49" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="57">
+      <c r="B49" s="56">
         <f>IF(B48&gt;=0,0,J11*ABS(B48))</f>
         <v>183.978500389397</v>
       </c>
       <c r="C49" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="D49" s="51">
+      <c r="D49" s="50">
         <f>D48/2+D27*H26*F25</f>
         <v>1357.73351302844</v>
       </c>
-      <c r="E49" s="58" t="str">
+      <c r="E49" s="57" t="str">
         <f>IF(B49&lt;D49,"验算通过","验算不通过")</f>
         <v>验算通过</v>
       </c>
-      <c r="F49" s="56"/>
-      <c r="G49" s="56"/>
-      <c r="H49" s="56"/>
+      <c r="F49" s="55"/>
+      <c r="G49" s="55"/>
+      <c r="H49" s="55"/>
     </row>
     <row r="50" ht="20.1" customHeight="1" spans="1:8">
       <c r="A50" s="36"/>
-      <c r="B50" s="57"/>
+      <c r="B50" s="56"/>
       <c r="C50" s="36"/>
-      <c r="D50" s="51"/>
-      <c r="E50" s="56"/>
-      <c r="F50" s="56"/>
-      <c r="G50" s="56"/>
-      <c r="H50" s="56"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="55"/>
+      <c r="F50" s="55"/>
+      <c r="G50" s="55"/>
+      <c r="H50" s="55"/>
     </row>
     <row r="51" ht="20.1" customHeight="1" spans="1:8">
-      <c r="A51" s="55" t="s">
+      <c r="A51" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="B51" s="56"/>
-      <c r="C51" s="56"/>
-      <c r="D51" s="56"/>
-      <c r="E51" s="56"/>
-      <c r="F51" s="56"/>
-      <c r="G51" s="56"/>
-      <c r="H51" s="56"/>
+      <c r="B51" s="55"/>
+      <c r="C51" s="55"/>
+      <c r="D51" s="55"/>
+      <c r="E51" s="55"/>
+      <c r="F51" s="55"/>
+      <c r="G51" s="55"/>
+      <c r="H51" s="55"/>
     </row>
     <row r="52" ht="20.1" customHeight="1" spans="1:8">
       <c r="A52" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="B52" s="57">
+      <c r="B52" s="56">
         <f>B8+24*H26*D25</f>
         <v>275.212059698439</v>
       </c>
       <c r="C52" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="D52" s="57">
+      <c r="D52" s="56">
         <f>SUM(O36:O45)+INDEX(Q36:Q45,H25)</f>
         <v>1691.73323833432</v>
       </c>
-      <c r="E52" s="56" t="s">
+      <c r="E52" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="F52" s="57">
+      <c r="F52" s="56">
         <f>IF(B25&lt;=0.8,0,24*H26*F25/2)</f>
         <v>554.17694409324</v>
       </c>
-      <c r="G52" s="56"/>
-      <c r="H52" s="56"/>
+      <c r="G52" s="55"/>
+      <c r="H52" s="55"/>
     </row>
     <row r="53" ht="20.1" customHeight="1" spans="1:8">
       <c r="A53" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="B53" s="57">
+      <c r="B53" s="56">
         <f>J11*(B52+F52)</f>
         <v>663.511203033343</v>
       </c>
       <c r="C53" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="D53" s="51">
+      <c r="D53" s="50">
         <f>D52/2</f>
         <v>845.866619167158</v>
       </c>
-      <c r="E53" s="58" t="str">
+      <c r="E53" s="57" t="str">
         <f>IF(B53&lt;D53,"验算通过","验算不通过")</f>
         <v>验算通过</v>
       </c>
-      <c r="F53" s="56"/>
-      <c r="G53" s="56"/>
-      <c r="H53" s="56"/>
+      <c r="F53" s="55"/>
+      <c r="G53" s="55"/>
+      <c r="H53" s="55"/>
     </row>
     <row r="54" ht="20.1" customHeight="1" spans="1:8">
       <c r="A54" s="36"/>
-      <c r="B54" s="57"/>
+      <c r="B54" s="56"/>
       <c r="C54" s="36"/>
-      <c r="D54" s="51"/>
-      <c r="E54" s="56"/>
-      <c r="F54" s="56"/>
-      <c r="G54" s="56"/>
-      <c r="H54" s="56"/>
+      <c r="D54" s="50"/>
+      <c r="E54" s="55"/>
+      <c r="F54" s="55"/>
+      <c r="G54" s="55"/>
+      <c r="H54" s="55"/>
     </row>
     <row r="55" ht="20.1" customHeight="1" spans="1:8">
-      <c r="A55" s="55" t="s">
+      <c r="A55" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="B55" s="57"/>
+      <c r="B55" s="56"/>
       <c r="C55" s="36"/>
-      <c r="D55" s="51"/>
-      <c r="E55" s="56"/>
-      <c r="F55" s="56"/>
-      <c r="G55" s="56"/>
-      <c r="H55" s="56"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="55"/>
+      <c r="F55" s="55"/>
+      <c r="G55" s="55"/>
+      <c r="H55" s="55"/>
     </row>
     <row r="56" ht="20.1" customHeight="1" spans="1:8">
       <c r="A56" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="B56" s="57" t="e">
+      <c r="B56" s="56" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="C56" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="D56" s="57" t="e">
+      <c r="D56" s="56" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
@@ -4042,7 +4086,7 @@
       <c r="G56" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="H56" s="59" t="e">
+      <c r="H56" s="58" t="e">
         <f>IF(B56&gt;0,IF(ABS(D56)&gt;0,"偏心受压","轴心受压"),IF(ABS(D56)&gt;0,"偏心受拉","轴心受拉"))</f>
         <v>#REF!</v>
       </c>
@@ -4051,28 +4095,28 @@
       <c r="A57" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="B57" s="57" t="e">
+      <c r="B57" s="56" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="C57" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="D57" s="57" t="e">
+      <c r="D57" s="56" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="E57" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="F57" s="51">
+      <c r="F57" s="50">
         <f>POWER(B25*1000,2)*PI()/4*F56</f>
         <v>6283.18530717959</v>
       </c>
       <c r="G57" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="H57" s="59" t="e">
+      <c r="H57" s="58" t="e">
         <f>IF(B57&gt;0,IF(ABS(D57)&gt;0,"偏心受压","轴心受压"),IF(ABS(D57)&gt;0,"偏心受拉","轴心受拉"))</f>
         <v>#REF!</v>
       </c>
@@ -4081,25 +4125,25 @@
       <c r="A58" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="B58" s="57" t="e">
+      <c r="B58" s="56" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="C58" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="D58" s="57" t="e">
+      <c r="D58" s="56" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="E58" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="F58" s="57" t="e">
+      <c r="F58" s="56" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="H58" s="60"/>
+      <c r="H58" s="59"/>
     </row>
     <row r="59" ht="20.1" customHeight="1" spans="1:8">
       <c r="A59" s="36" t="s">
@@ -4109,129 +4153,129 @@
         <f>POWER(D26,2)*PI()/4*B26</f>
         <v>27488.9357189107</v>
       </c>
-      <c r="C59" s="58" t="e">
+      <c r="C59" s="57" t="e">
         <f>IF(AND(B59&gt;F57,B59&gt;D58,B59&gt;B58,B59&gt;F58),"验算通过","验算不通过")</f>
         <v>#REF!</v>
       </c>
-      <c r="D59" s="57"/>
+      <c r="D59" s="56"/>
       <c r="E59" s="36"/>
       <c r="F59" s="36"/>
-      <c r="G59" s="58"/>
-      <c r="H59" s="60"/>
+      <c r="G59" s="57"/>
+      <c r="H59" s="59"/>
     </row>
     <row r="60" ht="20.1" customHeight="1" spans="1:8">
-      <c r="A60" s="55" t="s">
+      <c r="A60" s="54" t="s">
         <v>108</v>
       </c>
       <c r="C60" s="36"/>
-      <c r="D60" s="51"/>
-      <c r="E60" s="56"/>
-      <c r="F60" s="56"/>
-      <c r="G60" s="56"/>
-      <c r="H60" s="56"/>
+      <c r="D60" s="50"/>
+      <c r="E60" s="55"/>
+      <c r="F60" s="55"/>
+      <c r="G60" s="55"/>
+      <c r="H60" s="55"/>
     </row>
     <row r="61" ht="20.1" customHeight="1" spans="1:8">
-      <c r="A61" s="57" t="s">
+      <c r="A61" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="B61" s="57" t="e">
+      <c r="B61" s="56" t="e">
         <f>#REF!*1000</f>
         <v>#REF!</v>
       </c>
-      <c r="C61" s="57" t="s">
+      <c r="C61" s="56" t="s">
         <v>110</v>
       </c>
-      <c r="D61" s="51" t="e">
+      <c r="D61" s="50" t="e">
         <f>#REF!*1000</f>
         <v>#REF!</v>
       </c>
-      <c r="E61" s="56"/>
-      <c r="F61" s="56"/>
-      <c r="G61" s="56"/>
-      <c r="H61" s="56"/>
+      <c r="E61" s="55"/>
+      <c r="F61" s="55"/>
+      <c r="G61" s="55"/>
+      <c r="H61" s="55"/>
     </row>
     <row r="62" ht="20.1" customHeight="1" spans="1:8">
-      <c r="A62" s="57" t="s">
+      <c r="A62" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="B62" s="57">
+      <c r="B62" s="56">
         <v>10</v>
       </c>
-      <c r="C62" s="58" t="e">
+      <c r="C62" s="57" t="e">
         <f>IF(AND(B62&gt;B61,B62&gt;D61),"验算通过","验算不通过")</f>
         <v>#REF!</v>
       </c>
-      <c r="D62" s="51"/>
-      <c r="E62" s="56"/>
-      <c r="F62" s="56"/>
-      <c r="G62" s="56"/>
-      <c r="H62" s="56"/>
+      <c r="D62" s="50"/>
+      <c r="E62" s="55"/>
+      <c r="F62" s="55"/>
+      <c r="G62" s="55"/>
+      <c r="H62" s="55"/>
     </row>
     <row r="63" ht="20.1" customHeight="1" spans="1:9">
       <c r="A63" s="36"/>
-      <c r="B63" s="57"/>
+      <c r="B63" s="56"/>
       <c r="C63" s="36"/>
-      <c r="D63" s="51"/>
-      <c r="E63" s="56"/>
-      <c r="F63" s="56"/>
-      <c r="G63" s="56"/>
-      <c r="H63" s="56"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="55"/>
+      <c r="F63" s="55"/>
+      <c r="G63" s="55"/>
+      <c r="H63" s="55"/>
       <c r="I63" s="40"/>
     </row>
     <row r="64" ht="20.1" customHeight="1" spans="1:8">
-      <c r="A64" s="55" t="s">
+      <c r="A64" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="B64" s="58" t="e">
+      <c r="B64" s="57" t="e">
         <f>IF(AND(E49="验算通过",E53="验算通过",C59="验算通过",C62="验算通过"),"验算通过","验算不通过")</f>
         <v>#REF!</v>
       </c>
       <c r="C64" s="36"/>
       <c r="D64" s="36"/>
-      <c r="E64" s="56"/>
-      <c r="F64" s="56"/>
-      <c r="G64" s="56"/>
-      <c r="H64" s="56"/>
+      <c r="E64" s="55"/>
+      <c r="F64" s="55"/>
+      <c r="G64" s="55"/>
+      <c r="H64" s="55"/>
     </row>
     <row r="65" ht="20.1" customHeight="1" spans="1:8">
       <c r="A65" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="B65" s="58" t="e">
+      <c r="B65" s="57" t="e">
         <f>IF(B64="验算通过",B25,"验算不通过")</f>
         <v>#REF!</v>
       </c>
       <c r="C65" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="D65" s="58" t="e">
+      <c r="D65" s="57" t="e">
         <f>IF(B64="验算通过",D25+F25,"验算不通过")</f>
         <v>#REF!</v>
       </c>
-      <c r="E65" s="56"/>
-      <c r="F65" s="56"/>
-      <c r="G65" s="56"/>
-      <c r="H65" s="56"/>
+      <c r="E65" s="55"/>
+      <c r="F65" s="55"/>
+      <c r="G65" s="55"/>
+      <c r="H65" s="55"/>
     </row>
     <row r="66" ht="20.1" customHeight="1" spans="1:8">
       <c r="A66" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B66" s="58" t="e">
+      <c r="B66" s="57" t="e">
         <f>IF(B64="验算通过",B26,"验算不通过")</f>
         <v>#REF!</v>
       </c>
       <c r="C66" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="D66" s="58" t="e">
+      <c r="D66" s="57" t="e">
         <f>IF(B64="验算通过",D26,"验算不通过")</f>
         <v>#REF!</v>
       </c>
-      <c r="E66" s="56"/>
-      <c r="F66" s="56"/>
-      <c r="G66" s="56"/>
-      <c r="H66" s="56"/>
+      <c r="E66" s="55"/>
+      <c r="F66" s="55"/>
+      <c r="G66" s="55"/>
+      <c r="H66" s="55"/>
     </row>
     <row r="67" ht="20.1" customHeight="1"/>
     <row r="68" ht="20.1" customHeight="1" spans="1:5">
@@ -4255,29 +4299,58 @@
     <mergeCell ref="A68:E68"/>
   </mergeCells>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27">
-      <formula1>"是,否"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>"C20,C25,C30,C35,C40"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36:B38">
+      <formula1>"黏性土,粉土,砂土"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
+      <formula1>"HPB300,HRB400,HRB500"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H11">
       <formula1>"直线型,直转型,转角型,终端型"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>"C20,C25,C30,C35,C40"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
-      <formula1>"HPB300,HRB400,HRB500"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J26">
       <formula1>"嵌入岩层,支立于土上,支立于岩层"</formula1>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D13 F13 D23 F23 D11:D12 F11:F12"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36:B38">
-      <formula1>"黏性土,粉土,砂土"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27">
+      <formula1>"是,否"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2050" r:id="rId3" name="计算">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>11</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>11</xdr:col>
+                <xdr:colOff>1085850</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>247650</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2050" r:id="rId3" name="计算"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
 </worksheet>
 </file>
 
@@ -4286,7 +4359,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:W100"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>

</xml_diff>